<commit_message>
bump 1.0.1 -- orthographe
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -31,62 +31,46 @@
     <t xml:space="preserve">IntelliJeu (Crédit)</t>
   </si>
   <si>
-    <t xml:space="preserve">Conçu par (Textes et adaption): François-X. Lyonnet du Moutier &amp; Charles D.%n%nIntellijeu est basé sur le jeu Mécanicarte créé par Aurélien Lefrançois et Prismatik. Distribué sous la licence CC-BY-NC-SA. vous pouvez-partager, et adapter le jeu en le laissant sous la licences CC-BY-NC-SA, en citant les auteurs originaux et sans utilisation commerciale. Carte généré via Squib (licence MIT), et Icône de «Game Icon» (CC-BY 3.0)%n%nCode source :%nhttps://github.com/ixeft/intellijeu%nPour plus d’informations :%nhttps://intellijeu.fr%nVers.1.0.0</t>
+    <t xml:space="preserve">Conçu par (Textes et adaption): François-X. Lyonnet du Moutier &amp; Charles D.%n%nIntellijeu est basé sur le jeu Mécanicarte créé par Aurélien Lefrançois et Prismatik. Distribué sous la licence CC-BY-NC-SA. vous pouvez partager et adapter le jeu en le laissant sous la license CC-BY-NC-SA, en citant les auteurs originaux et sans utilisation commerciale. Carte générée via Squib (licence MIT), et Icône de «Game Icon» (CC-BY 3.0)%n%nCode source :%nhttps://github.com/ixeft/intellijeu%nPour plus d’informations :%nhttps://intellijeu.fr%nContact : contact@intellijeu.fr%nVers.1.0.1</t>
   </si>
   <si>
     <t xml:space="preserve">IntelliJeu</t>
   </si>
   <si>
-    <t xml:space="preserve">Intellijeu est un jeu de carte conçu pour t'aider à créer des grands jeux de qualité.%n Les cartes, diviser en 4 catégories te permettent de comprendre les mécaniques qui font d’un jeu, un jeu réussi.%n%nCompétences (15 cartes) :%nLes compétences utilisés par les participants durant le jeu%n%nMatériel (23 cartes) :%nLe matériel necessaire au bon déroulement du jeu%n%nMécaniques (19 cartes) :%nLes mécaniques régissant le jeu.%n%nTerrain (10 cartes) :%nLes terrains sur lequel le jeu se déroule.</t>
+    <t xml:space="preserve">Intellijeu est un jeu de cartes conçu pour t'aider à créer des grands jeux de qualité.%n Les cartes, divisées en 4 catégories, te permettent de comprendre les mécaniques qui font d’un jeu, un jeu réussi.%n%nCompétences (15 cartes) :%nLes compétences utilisés par les participants durant le jeu%n%nMatériel (23 cartes) :%nLe matériel necessaire au bon déroulement du jeu%n%nMécaniques (19 cartes) :%nLes mécaniques régissant le jeu.%n%nTerrain (10 cartes) :%nLe ou les terrains sur le(s)quel(s) le jeu se déroule.</t>
   </si>
   <si>
     <t xml:space="preserve">(1) Jouer à un jeu</t>
   </si>
   <si>
-    <t xml:space="preserve">Intellijeu peut s’utiliser pour comprendre comment fonctionne un jeu et l’améliorer%n%n Pour commencer on jeu à un grand jeu !%n%n1. Choisir un grand jeu, Ex : la tèque%n%n2. Expliquer les règles de ce jeu à tous%n%n3. Jouer au jeu</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(2) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Décomposer un jeu</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Se divisent en groupe de ~5 personnes%n%n2. Distribuer les cartes intellijeu entre les joueurs. Chaque joueur selectionne les cartes dans sa main qui semble correspondre au fonctionnement du jeu joué%n%n3. Chacun un son tour, les joueurs pose un carte et explique pourquoi elle correspond au jeu, les autres joueurs donne leur avis sur cette carte.%n%n4. Avec les cartes qui font consensus, on forme la «carte d’identité du jeu». Cette carte d’identité est subjective et correspondra à la vision du jeu par le groupe de joueur.</t>
+    <t xml:space="preserve">Intellijeu peut s’utiliser pour comprendre comment fonctionne un jeu et l’améliorer;%n%n Pour commencer on joue à un grand jeu !%n%n1. Choisir un grand jeu, Ex : la thèque%n%n2. Expliquer les règles de ce jeu à toutes et tous%n%n3. Jouer au jeu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2) Décomposer un jeu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Se divisent en groupe de ~5 personnes%n%n2. Distribuer les cartes intellijeu entre les joueurs. Chaque joueur selectionne les cartes dans sa main qui semblent correspondre au fonctionnement du jeu joué%n%n3. Chacun à son tour, les joueurs posent un carte et expliquent pourquoi elle correspond au jeu, les autres joueurs donnent leur avis sur cette carte.%n%n4. Avec les cartes qui font consensus, on forme la « carte d’identité du jeu ». Cette carte d’identité est subjective et correspond à la vision du jeu par le groupe de joueur.</t>
   </si>
   <si>
     <t xml:space="preserve">(3) Créer une variante</t>
   </si>
   <si>
-    <t xml:space="preserve">Lorsque les joueurs se sont mise d’accord sur une analyse.%n%n1. On choisi une carte qui ne fait pas partie de la caret d’identité du jeu%n%n2. On essaie de modifier le grand jeu pour rajouter la nouvelle carte %n%n3. On teste la variante pour voir si ça fonctionne</t>
+    <t xml:space="preserve">Lorsque les joueurs se sont mis d’accord sur une analyse.%n%n1. On choisit une carte qui ne fait pas partie de la carte d’identité du jeu%n%n2. On essaie de modifier le grand jeu pour rajouter la nouvelle carte %n%n3. On teste la variante pour voir si ça fonctionne;</t>
   </si>
   <si>
     <t xml:space="preserve">(4) Créer un jeu</t>
   </si>
   <si>
-    <t xml:space="preserve">Bien compris comment utiliser intellijeu ? Les mécaniques de jeux n’ont pas de secret ? Il est temps de créer un jeu tout neuf !%n%n1. Choisir 3 cartes, soit au hasard, soit des éléments avec lesquelles vous voulez travailler. Vous avez ainsi choisi vos contraintes créatives%n%n2. Éventuellement, choisissez une carte maitresse qui sera votre contrainte principale%n%n3. Utiliser ces contrainte comme base pour créer votre jeu.%n%n4. Si vous bloquez, vous pouvez éliminer une carte trop difficile, ou en ajouter une.</t>
+    <t xml:space="preserve">Bien compris comment utiliser intellijeu ? Les mécaniques de jeux n’ont pas de secret ? Il est temps de créer un jeu tout neuf !%n%n1. Choisir 3 cartes, soit au hasard, soit des éléments avec lesquels vous voulez de travailler. Vous avez ainsi choisi vos contraintes créatives%n%n2. Éventuellement, choisissez une carte maitresse qui sera votre contrainte principale%n%n3. Utiliser ces contraintes pour créer votre jeu.%n%n4. Si vous bloquez, vous pouvez éliminer une carte trop difficile, ou en ajouter une.</t>
   </si>
   <si>
     <t xml:space="preserve">Autres petits jeux</t>
   </si>
   <si>
-    <t xml:space="preserve">%n%nTrouve le jeu ! (3 à 6 Joueurs)%n%n1. Un joueur choisi un grand jeu dans sa tête et le garde secret.%n%n2. Le joueur décompose le jeu avec intellijeu%n%n3. Le joueur pose les cartes face visible devant les autres joueurs de la plus représentative du jeu à la moins proche.%n%n4. Les autres joueurs essaye de deviner le jeu choisi. Le premier à trouver a gagné et choisi à son tour un grand jeu mystère.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%n%nRoulette ludique (2 à 6 Joueurs)%n%n On tire une carte intellijeu, le premier à donner le nom d’un jeu qui utilise cette carte gagne un point !%n%nChabadabajeu (2 à 30 joueurs)%n%n1.On forme des équipes.%n%n2. On tire une carte%n%n3. Chacune à leur tour les équipes cherchent un grand jeu qui utilise cette carte. La dernière équipe à trouver un grand jeu gagne la manche.</t>
+    <t xml:space="preserve">%n%nTrouve le jeu ! (3 à 6 Joueurs)%n%n1. Un joueur choisit un grand jeu dans sa tête et le garde secret.%n%n2. Le joueur décompose le jeu avec intellijeu%n%n3. Le joueur pose les cartes face visible devant les autres joueurs de la plus représentative du jeu à la plus éloignée.%n%n4. Les autres joueurs essaient de deviner le jeu choisi. Le premier à trouver a gagné et choisit à son tour un grand jeu mystère.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%n%nRoulette ludique (2 à 6 Joueurs)%n%n On tire une carte intellijeu, le premier à donner le nom d’un jeu qui utilise cette carte gagne un point !%n%nChabadabajeu (2 à 30 joueurs)%n%n1.On forme des équipes.%n%n2. On tire une carte%n%n3. Chacune à leur tour, les équipes cherchent un grand jeu qui utilise cette carte. La dernière équipe à trouver un grand jeu gagne la manche.</t>
   </si>
 </sst>
 </file>
@@ -96,7 +80,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -123,11 +107,6 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,15 +151,11 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -195,30 +170,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -346,62 +297,62 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="60.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="60.74"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="114.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="145.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" s="10" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+    <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -409,15 +360,15 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -425,7 +376,7 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>